<commit_message>
rejection data pushed DF
</commit_message>
<xml_diff>
--- a/conditions/SocaMRIConditions_Version1A_Run1.xlsx
+++ b/conditions/SocaMRIConditions_Version1A_Run1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>Cue</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>stim/WWmale23-3happy_edited.jpg</t>
+  </si>
+  <si>
+    <t>stim/WWmale21-3happy_edited.jpg</t>
   </si>
 </sst>
 </file>
@@ -606,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="89" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1048,7 +1051,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>

</xml_diff>